<commit_message>
combine data based on gold_spot and format to monthly since 2006
</commit_message>
<xml_diff>
--- a/Data/Gold_price_averages_in_a range_of_currencies_since_1978.xlsx
+++ b/Data/Gold_price_averages_in_a range_of_currencies_since_1978.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khanh\Documents\GreenWich\COMP1682.1 Final Project 1\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C5C365-2833-4112-A50E-49DE0B57C314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA3FC31-8755-4429-9B30-41708AD48CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{9DE83BEB-DC61-4378-A362-8D4111DA83C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9DE83BEB-DC61-4378-A362-8D4111DA83C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="2" r:id="rId1"/>

</xml_diff>